<commit_message>
Oyvinds verson som funker med 4 grupper
</commit_message>
<xml_diff>
--- a/Old Model/Input/model_input_9groups.xlsx
+++ b/Old Model/Input/model_input_9groups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oyvindasplin/Documents/Indok/NTNU/Optimering/Master V22/master2022/Old Model/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081CD192-B9B0-7842-9FB1-8DAEE56EA12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661712D6-97CC-C044-8DA9-D10331D81991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="540" windowWidth="38400" windowHeight="19260" xr2:uid="{A5361B1D-8409-0845-981B-BA630B7E70E6}"/>
+    <workbookView xWindow="1020" yWindow="500" windowWidth="38400" windowHeight="19260" xr2:uid="{A5361B1D-8409-0845-981B-BA630B7E70E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="14" r:id="rId1"/>
@@ -1118,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1975E0D-6F6E-A842-BF84-34A209557AB1}">
-  <dimension ref="A1:BX29"/>
+  <dimension ref="A1:DG61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AM22" sqref="AM22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1139,9 +1139,11 @@
     <col min="44" max="71" width="3.5" customWidth="1"/>
     <col min="72" max="72" width="10.83203125" customWidth="1"/>
     <col min="74" max="74" width="4.33203125" customWidth="1"/>
+    <col min="83" max="83" width="10.33203125" customWidth="1"/>
+    <col min="84" max="139" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:111" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="21" t="s">
         <v>133</v>
       </c>
@@ -1357,7 +1359,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:76" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:111" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="30">
         <v>0.1</v>
@@ -1379,88 +1381,88 @@
         <v>33</v>
       </c>
       <c r="I2" s="27">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="J2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="K2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="L2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="M2" s="28">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="N2" s="28">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="O2" s="28">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="P2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="Q2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="R2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="S2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="T2" s="28">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="U2" s="28">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="V2" s="28">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="W2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="X2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="Y2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="Z2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="AA2" s="28">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="AB2" s="28">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="AC2" s="28">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="AD2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="AE2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="AF2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="AG2" s="28">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="AH2" s="28">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="AI2" s="28">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="AJ2" s="29">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="AK2" s="47">
         <v>20</v>
@@ -1574,8 +1576,93 @@
         <v>450</v>
       </c>
       <c r="BX2" s="2"/>
-    </row>
-    <row r="3" spans="1:76" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="CD2" s="3"/>
+      <c r="CF2">
+        <v>60</v>
+      </c>
+      <c r="CG2">
+        <v>60</v>
+      </c>
+      <c r="CH2">
+        <v>60</v>
+      </c>
+      <c r="CI2">
+        <v>60</v>
+      </c>
+      <c r="CJ2">
+        <v>49</v>
+      </c>
+      <c r="CK2">
+        <v>49</v>
+      </c>
+      <c r="CL2">
+        <v>49</v>
+      </c>
+      <c r="CM2">
+        <v>60</v>
+      </c>
+      <c r="CN2">
+        <v>60</v>
+      </c>
+      <c r="CO2">
+        <v>60</v>
+      </c>
+      <c r="CP2">
+        <v>60</v>
+      </c>
+      <c r="CQ2">
+        <v>49</v>
+      </c>
+      <c r="CR2">
+        <v>49</v>
+      </c>
+      <c r="CS2">
+        <v>49</v>
+      </c>
+      <c r="CT2">
+        <v>60</v>
+      </c>
+      <c r="CU2">
+        <v>60</v>
+      </c>
+      <c r="CV2">
+        <v>60</v>
+      </c>
+      <c r="CW2">
+        <v>60</v>
+      </c>
+      <c r="CX2">
+        <v>49</v>
+      </c>
+      <c r="CY2">
+        <v>49</v>
+      </c>
+      <c r="CZ2">
+        <v>49</v>
+      </c>
+      <c r="DA2">
+        <v>60</v>
+      </c>
+      <c r="DB2">
+        <v>60</v>
+      </c>
+      <c r="DC2">
+        <v>60</v>
+      </c>
+      <c r="DD2">
+        <v>60</v>
+      </c>
+      <c r="DE2">
+        <v>49</v>
+      </c>
+      <c r="DF2">
+        <v>49</v>
+      </c>
+      <c r="DG2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:111" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="59"/>
       <c r="C3" s="59"/>
@@ -1587,88 +1674,88 @@
         <v>44</v>
       </c>
       <c r="I3" s="14">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="J3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="K3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="L3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="M3" s="15">
-        <v>3.468</v>
+        <v>6</v>
       </c>
       <c r="N3" s="15">
-        <v>3.468</v>
+        <v>6</v>
       </c>
       <c r="O3" s="15">
-        <v>3.468</v>
+        <v>6</v>
       </c>
       <c r="P3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="Q3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="R3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="S3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="T3" s="15">
-        <v>3.468</v>
+        <v>6</v>
       </c>
       <c r="U3" s="15">
-        <v>3.468</v>
+        <v>6</v>
       </c>
       <c r="V3" s="15">
-        <v>3.468</v>
+        <v>6</v>
       </c>
       <c r="W3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="X3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="Y3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="Z3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="AA3" s="15">
-        <v>3.468</v>
+        <v>6</v>
       </c>
       <c r="AB3" s="15">
-        <v>3.468</v>
+        <v>6</v>
       </c>
       <c r="AC3" s="15">
-        <v>3.468</v>
+        <v>6</v>
       </c>
       <c r="AD3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="AE3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="AF3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="AG3" s="15">
-        <v>6.3579999999999997</v>
+        <v>11</v>
       </c>
       <c r="AH3" s="15">
-        <v>3.468</v>
+        <v>6</v>
       </c>
       <c r="AI3" s="15">
-        <v>3.468</v>
+        <v>6</v>
       </c>
       <c r="AJ3" s="16">
-        <v>3.468</v>
+        <v>6</v>
       </c>
       <c r="AK3" s="48">
         <v>2</v>
@@ -1782,8 +1869,93 @@
         <v>450</v>
       </c>
       <c r="BX3" s="2"/>
-    </row>
-    <row r="4" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD3" s="3"/>
+      <c r="CF3">
+        <v>11</v>
+      </c>
+      <c r="CG3">
+        <v>11</v>
+      </c>
+      <c r="CH3">
+        <v>11</v>
+      </c>
+      <c r="CI3">
+        <v>11</v>
+      </c>
+      <c r="CJ3">
+        <v>6</v>
+      </c>
+      <c r="CK3">
+        <v>6</v>
+      </c>
+      <c r="CL3">
+        <v>6</v>
+      </c>
+      <c r="CM3">
+        <v>11</v>
+      </c>
+      <c r="CN3">
+        <v>11</v>
+      </c>
+      <c r="CO3">
+        <v>11</v>
+      </c>
+      <c r="CP3">
+        <v>11</v>
+      </c>
+      <c r="CQ3">
+        <v>6</v>
+      </c>
+      <c r="CR3">
+        <v>6</v>
+      </c>
+      <c r="CS3">
+        <v>6</v>
+      </c>
+      <c r="CT3">
+        <v>11</v>
+      </c>
+      <c r="CU3">
+        <v>11</v>
+      </c>
+      <c r="CV3">
+        <v>11</v>
+      </c>
+      <c r="CW3">
+        <v>11</v>
+      </c>
+      <c r="CX3">
+        <v>6</v>
+      </c>
+      <c r="CY3">
+        <v>6</v>
+      </c>
+      <c r="CZ3">
+        <v>6</v>
+      </c>
+      <c r="DA3">
+        <v>11</v>
+      </c>
+      <c r="DB3">
+        <v>11</v>
+      </c>
+      <c r="DC3">
+        <v>11</v>
+      </c>
+      <c r="DD3">
+        <v>11</v>
+      </c>
+      <c r="DE3">
+        <v>6</v>
+      </c>
+      <c r="DF3">
+        <v>6</v>
+      </c>
+      <c r="DG3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -1930,8 +2102,9 @@
         <v>450</v>
       </c>
       <c r="BX4" s="2"/>
-    </row>
-    <row r="5" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD4" s="3"/>
+    </row>
+    <row r="5" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -2078,8 +2251,93 @@
         <v>450</v>
       </c>
       <c r="BX5" s="2"/>
-    </row>
-    <row r="6" spans="1:76" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="CD5" s="3"/>
+      <c r="CF5">
+        <v>32</v>
+      </c>
+      <c r="CG5">
+        <v>32</v>
+      </c>
+      <c r="CH5">
+        <v>32</v>
+      </c>
+      <c r="CI5">
+        <v>32</v>
+      </c>
+      <c r="CJ5">
+        <v>28</v>
+      </c>
+      <c r="CK5">
+        <v>28</v>
+      </c>
+      <c r="CL5">
+        <v>28</v>
+      </c>
+      <c r="CM5">
+        <v>32</v>
+      </c>
+      <c r="CN5">
+        <v>32</v>
+      </c>
+      <c r="CO5">
+        <v>32</v>
+      </c>
+      <c r="CP5">
+        <v>32</v>
+      </c>
+      <c r="CQ5">
+        <v>28</v>
+      </c>
+      <c r="CR5">
+        <v>28</v>
+      </c>
+      <c r="CS5">
+        <v>28</v>
+      </c>
+      <c r="CT5">
+        <v>32</v>
+      </c>
+      <c r="CU5">
+        <v>32</v>
+      </c>
+      <c r="CV5">
+        <v>32</v>
+      </c>
+      <c r="CW5">
+        <v>32</v>
+      </c>
+      <c r="CX5">
+        <v>28</v>
+      </c>
+      <c r="CY5">
+        <v>28</v>
+      </c>
+      <c r="CZ5">
+        <v>28</v>
+      </c>
+      <c r="DA5">
+        <v>32</v>
+      </c>
+      <c r="DB5">
+        <v>32</v>
+      </c>
+      <c r="DC5">
+        <v>32</v>
+      </c>
+      <c r="DD5">
+        <v>32</v>
+      </c>
+      <c r="DE5">
+        <v>28</v>
+      </c>
+      <c r="DF5">
+        <v>28</v>
+      </c>
+      <c r="DG5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:111" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -2226,8 +2484,93 @@
         <v>450</v>
       </c>
       <c r="BX6" s="2"/>
-    </row>
-    <row r="7" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD6" s="3"/>
+      <c r="CF6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="CG6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="CH6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="CI6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="CJ6">
+        <v>3.468</v>
+      </c>
+      <c r="CK6">
+        <v>3.468</v>
+      </c>
+      <c r="CL6">
+        <v>3.468</v>
+      </c>
+      <c r="CM6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="CN6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="CO6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="CP6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="CQ6">
+        <v>3.468</v>
+      </c>
+      <c r="CR6">
+        <v>3.468</v>
+      </c>
+      <c r="CS6">
+        <v>3.468</v>
+      </c>
+      <c r="CT6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="CU6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="CV6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="CW6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="CX6">
+        <v>3.468</v>
+      </c>
+      <c r="CY6">
+        <v>3.468</v>
+      </c>
+      <c r="CZ6">
+        <v>3.468</v>
+      </c>
+      <c r="DA6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="DB6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="DC6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="DD6">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="DE6">
+        <v>3.468</v>
+      </c>
+      <c r="DF6">
+        <v>3.468</v>
+      </c>
+      <c r="DG6">
+        <v>3.468</v>
+      </c>
+    </row>
+    <row r="7" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="59"/>
       <c r="C7" s="59"/>
@@ -2314,8 +2657,9 @@
         <v>0</v>
       </c>
       <c r="BX7" s="2"/>
-    </row>
-    <row r="8" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD7" s="3"/>
+    </row>
+    <row r="8" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -2402,8 +2746,9 @@
         <v>0</v>
       </c>
       <c r="BX8" s="2"/>
-    </row>
-    <row r="9" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD8" s="3"/>
+    </row>
+    <row r="9" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="59"/>
       <c r="C9" s="59"/>
@@ -2490,8 +2835,9 @@
         <v>450</v>
       </c>
       <c r="BX9" s="2"/>
-    </row>
-    <row r="10" spans="1:76" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="CD9" s="3"/>
+    </row>
+    <row r="10" spans="1:111" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="59"/>
       <c r="C10" s="59"/>
@@ -2578,8 +2924,9 @@
         <v>450</v>
       </c>
       <c r="BX10" s="2"/>
-    </row>
-    <row r="11" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD10" s="3"/>
+    </row>
+    <row r="11" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="59"/>
       <c r="C11" s="59"/>
@@ -2660,8 +3007,9 @@
         <v>450</v>
       </c>
       <c r="BX11" s="2"/>
-    </row>
-    <row r="12" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD11" s="3"/>
+    </row>
+    <row r="12" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="59"/>
       <c r="C12" s="59"/>
@@ -2742,8 +3090,9 @@
         <v>450</v>
       </c>
       <c r="BX12" s="2"/>
-    </row>
-    <row r="13" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD12" s="3"/>
+    </row>
+    <row r="13" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="59"/>
       <c r="C13" s="59"/>
@@ -2824,8 +3173,9 @@
         <v>450</v>
       </c>
       <c r="BX13" s="2"/>
-    </row>
-    <row r="14" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD13" s="3"/>
+    </row>
+    <row r="14" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="59"/>
       <c r="C14" s="59"/>
@@ -2906,8 +3256,9 @@
         <v>0</v>
       </c>
       <c r="BX14" s="2"/>
-    </row>
-    <row r="15" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD14" s="3"/>
+    </row>
+    <row r="15" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="59"/>
       <c r="C15" s="59"/>
@@ -2988,8 +3339,9 @@
         <v>0</v>
       </c>
       <c r="BX15" s="2"/>
-    </row>
-    <row r="16" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD15" s="3"/>
+    </row>
+    <row r="16" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="59"/>
       <c r="C16" s="59"/>
@@ -3070,8 +3422,9 @@
         <v>450</v>
       </c>
       <c r="BX16" s="2"/>
-    </row>
-    <row r="17" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD16" s="3"/>
+    </row>
+    <row r="17" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="59"/>
       <c r="C17" s="59"/>
@@ -3152,8 +3505,9 @@
         <v>450</v>
       </c>
       <c r="BX17" s="2"/>
-    </row>
-    <row r="18" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD17" s="3"/>
+    </row>
+    <row r="18" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="59"/>
       <c r="C18" s="59"/>
@@ -3234,8 +3588,9 @@
         <v>450</v>
       </c>
       <c r="BX18" s="2"/>
-    </row>
-    <row r="19" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD18" s="3"/>
+    </row>
+    <row r="19" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="59"/>
       <c r="C19" s="59"/>
@@ -3316,8 +3671,9 @@
         <v>450</v>
       </c>
       <c r="BX19" s="2"/>
-    </row>
-    <row r="20" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD19" s="3"/>
+    </row>
+    <row r="20" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="59"/>
       <c r="C20" s="59"/>
@@ -3398,8 +3754,9 @@
         <v>450</v>
       </c>
       <c r="BX20" s="2"/>
-    </row>
-    <row r="21" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD20" s="3"/>
+    </row>
+    <row r="21" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="59"/>
       <c r="C21" s="59"/>
@@ -3480,8 +3837,9 @@
         <v>0</v>
       </c>
       <c r="BX21" s="2"/>
-    </row>
-    <row r="22" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD21" s="3"/>
+    </row>
+    <row r="22" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="59"/>
       <c r="C22" s="59"/>
@@ -3562,8 +3920,9 @@
         <v>0</v>
       </c>
       <c r="BX22" s="2"/>
-    </row>
-    <row r="23" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD22" s="3"/>
+    </row>
+    <row r="23" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="59"/>
       <c r="C23" s="59"/>
@@ -3644,8 +4003,9 @@
         <v>450</v>
       </c>
       <c r="BX23" s="2"/>
-    </row>
-    <row r="24" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD23" s="3"/>
+    </row>
+    <row r="24" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="59"/>
       <c r="C24" s="59"/>
@@ -3726,8 +4086,9 @@
         <v>450</v>
       </c>
       <c r="BX24" s="2"/>
-    </row>
-    <row r="25" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD24" s="3"/>
+    </row>
+    <row r="25" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="59"/>
       <c r="C25" s="59"/>
@@ -3808,8 +4169,9 @@
         <v>450</v>
       </c>
       <c r="BX25" s="2"/>
-    </row>
-    <row r="26" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD25" s="3"/>
+    </row>
+    <row r="26" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="59"/>
       <c r="C26" s="59"/>
@@ -3890,8 +4252,9 @@
         <v>450</v>
       </c>
       <c r="BX26" s="2"/>
-    </row>
-    <row r="27" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD26" s="3"/>
+    </row>
+    <row r="27" spans="1:82" x14ac:dyDescent="0.2">
       <c r="B27" s="24"/>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
@@ -3970,8 +4333,9 @@
       <c r="BW27" s="9">
         <v>450</v>
       </c>
-    </row>
-    <row r="28" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="CD27" s="3"/>
+    </row>
+    <row r="28" spans="1:82" x14ac:dyDescent="0.2">
       <c r="B28" s="24"/>
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
@@ -4050,14 +4414,112 @@
       <c r="BW28" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:76" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="CD28" s="3"/>
+    </row>
+    <row r="29" spans="1:82" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="BV29" s="8">
         <v>28</v>
       </c>
       <c r="BW29" s="10">
         <v>0</v>
       </c>
+      <c r="CD29" s="3"/>
+    </row>
+    <row r="30" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="CD30" s="3"/>
+    </row>
+    <row r="31" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="CD31" s="3"/>
+    </row>
+    <row r="32" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="CD32" s="3"/>
+    </row>
+    <row r="33" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD33" s="3"/>
+    </row>
+    <row r="34" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD34" s="3"/>
+    </row>
+    <row r="35" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD35" s="3"/>
+    </row>
+    <row r="36" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD36" s="3"/>
+    </row>
+    <row r="37" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD37" s="3"/>
+    </row>
+    <row r="38" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD38" s="3"/>
+    </row>
+    <row r="39" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD39" s="3"/>
+    </row>
+    <row r="40" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD40" s="3"/>
+    </row>
+    <row r="41" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD41" s="3"/>
+    </row>
+    <row r="42" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD42" s="3"/>
+    </row>
+    <row r="43" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD43" s="3"/>
+    </row>
+    <row r="44" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD44" s="3"/>
+    </row>
+    <row r="45" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD45" s="3"/>
+    </row>
+    <row r="46" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD46" s="3"/>
+    </row>
+    <row r="47" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD47" s="3"/>
+    </row>
+    <row r="48" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD48" s="3"/>
+    </row>
+    <row r="49" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD49" s="3"/>
+    </row>
+    <row r="50" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD50" s="3"/>
+    </row>
+    <row r="51" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD51" s="3"/>
+    </row>
+    <row r="52" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD52" s="3"/>
+    </row>
+    <row r="53" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD53" s="3"/>
+    </row>
+    <row r="54" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD54" s="3"/>
+    </row>
+    <row r="55" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD55" s="3"/>
+    </row>
+    <row r="56" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD56" s="3"/>
+    </row>
+    <row r="57" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD57" s="3"/>
+    </row>
+    <row r="58" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD58" s="3"/>
+    </row>
+    <row r="59" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD59" s="3"/>
+    </row>
+    <row r="60" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD60" s="3"/>
+    </row>
+    <row r="61" spans="82:82" x14ac:dyDescent="0.2">
+      <c r="CD61" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>